<commit_message>
add folder structure to CI List
</commit_message>
<xml_diff>
--- a/Project Management/PM_CI_List.xlsx
+++ b/Project Management/PM_CI_List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>File Name</t>
   </si>
@@ -42,15 +42,9 @@
     <t>Aya Mostafa</t>
   </si>
   <si>
-    <t>Customer</t>
-  </si>
-  <si>
     <t>REQ_SIQ</t>
   </si>
   <si>
-    <t>Dena</t>
-  </si>
-  <si>
     <t>PM_Review_Sheet</t>
   </si>
   <si>
@@ -63,18 +57,9 @@
     <t>REQ_Response_To_SIQ</t>
   </si>
   <si>
-    <t>Project Management/REQ_Response_To_SIQ.docx</t>
-  </si>
-  <si>
     <t>Project Management/PM_ReviewSheet.docx</t>
   </si>
   <si>
-    <t>Project Management/REQ_SIQ.docx</t>
-  </si>
-  <si>
-    <t>Project Management/REQ_CustomerReq.docx</t>
-  </si>
-  <si>
     <t>PM_IssueLog</t>
   </si>
   <si>
@@ -85,13 +70,40 @@
   </si>
   <si>
     <t>Project Management/PM_Coaching_Review.docx</t>
+  </si>
+  <si>
+    <t>Project Management</t>
+  </si>
+  <si>
+    <t>Requirement</t>
+  </si>
+  <si>
+    <t>Requirement/REQ_SIQ.docx</t>
+  </si>
+  <si>
+    <t>Requirement/REQ_CustomerReq.docx</t>
+  </si>
+  <si>
+    <t>Requirement/REQ_Response_To_SIQ.docx</t>
+  </si>
+  <si>
+    <t>Folder Structure</t>
+  </si>
+  <si>
+    <t>Sara Hassan</t>
+  </si>
+  <si>
+    <t>Sohila Abdalla</t>
+  </si>
+  <si>
+    <t>Dena Galal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -102,18 +114,45 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -142,7 +181,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -165,20 +204,71 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,125 +487,202 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Y8"/>
+  <dimension ref="A1:Z14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="19.77734375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="49.77734375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="12.6640625" style="3"/>
+    <col min="1" max="1" width="37.21875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="59.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:26" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-    </row>
-    <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
+    </row>
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="5"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="5"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+    </row>
+    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="C13" s="9"/>
+      <c r="D13" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="E13" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A8:A14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Add Branching strategy and edit CIL
</commit_message>
<xml_diff>
--- a/Project Management/PM_CI_List.xlsx
+++ b/Project Management/PM_CI_List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>File Name</t>
   </si>
@@ -97,13 +97,28 @@
   </si>
   <si>
     <t>Dena Galal</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V1.4 </t>
+  </si>
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>V1.3</t>
+  </si>
+  <si>
+    <t>V1.4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -154,6 +169,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -245,18 +268,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -267,6 +281,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -490,7 +519,7 @@
   <dimension ref="A1:Z14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -498,185 +527,214 @@
     <col min="1" max="1" width="37.21875" style="1" customWidth="1"/>
     <col min="2" max="2" width="38.5546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="28.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="59.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="12.6640625" style="1"/>
+    <col min="4" max="4" width="51.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:26" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="9"/>
+      <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="10" t="s">
+      <c r="C3" s="6"/>
+      <c r="D3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="8" t="s">
+      <c r="A4" s="9"/>
+      <c r="B4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="10" t="s">
+      <c r="C4" s="6"/>
+      <c r="D4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="8" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="10" t="s">
+      <c r="C5" s="6"/>
+      <c r="D5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="5"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="5"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="8" t="s">
+      <c r="A11" s="9"/>
+      <c r="B11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="10" t="s">
+      <c r="C11" s="6"/>
+      <c r="D11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="8" t="s">
+      <c r="A12" s="9"/>
+      <c r="B12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="8" t="s">
+      <c r="C12" s="6"/>
+      <c r="D12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="8" t="s">
+      <c r="A13" s="9"/>
+      <c r="B13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="10" t="s">
+      <c r="C13" s="6"/>
+      <c r="D13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="F14" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Add RTM to CIList
</commit_message>
<xml_diff>
--- a/Project Management/PM_CI_List.xlsx
+++ b/Project Management/PM_CI_List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>File Name</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Requirement/REQ_CustomerReq.docx</t>
   </si>
   <si>
-    <t>Requirement/REQ_Response_To_SIQ.docx</t>
-  </si>
-  <si>
     <t>Folder Structure</t>
   </si>
   <si>
@@ -102,23 +99,44 @@
     <t>Version</t>
   </si>
   <si>
-    <t xml:space="preserve">V1.4 </t>
-  </si>
-  <si>
     <t>V1</t>
   </si>
   <si>
-    <t>V1.3</t>
-  </si>
-  <si>
-    <t>V1.4</t>
+    <t>https://github.com/sohilaabdallaa/Internal-Banking-System/blob/main/Project%20Management/PM_Coaching_Review.xlsx</t>
+  </si>
+  <si>
+    <t>https://github.com/sohilaabdallaa/Internal-Banking-System/blob/main/Project%20Management/PM_IssueLog.xlsx</t>
+  </si>
+  <si>
+    <t>https://github.com/sohilaabdallaa/Internal-Banking-System/blob/main/Project%20Management/PM_PMP.docx</t>
+  </si>
+  <si>
+    <t>REQ_RTM</t>
+  </si>
+  <si>
+    <t>https://github.com/sohilaabdallaa/Internal-Banking-System/blob/main/Requirement/REC_RTM.xlsx</t>
+  </si>
+  <si>
+    <t>Requirement/REQ_RTM.docx</t>
+  </si>
+  <si>
+    <t>V2.1</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/sohilaabdallaa/Internal-Banking-System/blob/main/Requirement/REQ_SIQ.xlsx </t>
+  </si>
+  <si>
+    <t>https://github.com/sohilaabdallaa/Internal-Banking-System/blob/main/Requirement/REQ_Customer_Reqs.xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -177,6 +195,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -265,10 +290,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -283,6 +309,12 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -292,14 +324,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -519,7 +547,7 @@
   <dimension ref="A1:Z14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -528,14 +556,14 @@
     <col min="2" max="2" width="38.5546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="28.88671875" style="1" customWidth="1"/>
     <col min="4" max="4" width="51.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" style="8" customWidth="1"/>
     <col min="6" max="6" width="17.6640625" style="1" customWidth="1"/>
     <col min="7" max="16384" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -547,7 +575,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>3</v>
@@ -574,25 +602,27 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="6"/>
+      <c r="C2" s="13" t="s">
+        <v>29</v>
+      </c>
       <c r="D2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>27</v>
+      <c r="E2" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
+      <c r="A3" s="11"/>
       <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
@@ -600,40 +630,44 @@
       <c r="D3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>28</v>
+      <c r="E3" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="13" t="s">
+        <v>28</v>
+      </c>
       <c r="D4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>28</v>
+      <c r="E4" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="D5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>28</v>
+      <c r="E5" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>6</v>
@@ -644,7 +678,7 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
-      <c r="E6" s="12"/>
+      <c r="E6" s="9"/>
       <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -652,88 +686,103 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
-      <c r="E7" s="12"/>
+      <c r="E7" s="9"/>
       <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
-      <c r="E8" s="12"/>
+      <c r="E8" s="9"/>
       <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
-      <c r="E9" s="12"/>
+      <c r="E9" s="9"/>
       <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
+      <c r="A10" s="11"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="12"/>
+      <c r="E10" s="9"/>
       <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
+      <c r="A11" s="11"/>
       <c r="B11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="6"/>
+      <c r="C11" s="13" t="s">
+        <v>36</v>
+      </c>
       <c r="D11" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>29</v>
+        <v>19</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="6"/>
+      <c r="C12" s="13" t="s">
+        <v>36</v>
+      </c>
       <c r="D12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="12" t="s">
-        <v>28</v>
+      <c r="E12" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
+      <c r="A13" s="11"/>
       <c r="B13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="6"/>
+      <c r="C13" s="13" t="s">
+        <v>35</v>
+      </c>
       <c r="D13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
+      <c r="C14" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>33</v>
+      </c>
       <c r="F14" s="6"/>
     </row>
   </sheetData>
@@ -741,7 +790,16 @@
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A8:A14"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="C5" r:id="rId3"/>
+    <hyperlink ref="C14" r:id="rId4"/>
+    <hyperlink ref="C13" r:id="rId5"/>
+    <hyperlink ref="C12" r:id="rId6"/>
+    <hyperlink ref="C11" r:id="rId7"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add links for files in CIList
</commit_message>
<xml_diff>
--- a/Project Management/PM_CI_List.xlsx
+++ b/Project Management/PM_CI_List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>File Name</t>
   </si>
@@ -45,18 +45,12 @@
     <t>REQ_SIQ</t>
   </si>
   <si>
-    <t>PM_Review_Sheet</t>
-  </si>
-  <si>
     <t>Mayar Elhussieny</t>
   </si>
   <si>
     <t>REQ_Customer_Req</t>
   </si>
   <si>
-    <t>REQ_Response_To_SIQ</t>
-  </si>
-  <si>
     <t>Project Management/PM_ReviewSheet.docx</t>
   </si>
   <si>
@@ -93,9 +87,6 @@
     <t>Sohila Abdalla</t>
   </si>
   <si>
-    <t>Dena Galal</t>
-  </si>
-  <si>
     <t>Version</t>
   </si>
   <si>
@@ -130,6 +121,9 @@
   </si>
   <si>
     <t>https://github.com/sohilaabdallaa/Internal-Banking-System/blob/main/Requirement/REQ_Customer_Reqs.xlsx</t>
+  </si>
+  <si>
+    <t>PM_Peer_Review</t>
   </si>
 </sst>
 </file>
@@ -315,6 +309,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -324,7 +319,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -546,8 +540,8 @@
   </sheetPr>
   <dimension ref="A1:Z14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -563,7 +557,7 @@
   <sheetData>
     <row r="1" spans="1:26" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -575,7 +569,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>3</v>
@@ -602,72 +596,72 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>17</v>
+      <c r="A2" s="11" t="s">
+        <v>15</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>29</v>
+      <c r="C2" s="10" t="s">
+        <v>26</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
+      <c r="A3" s="12"/>
       <c r="B3" s="5" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>16</v>
-      </c>
       <c r="E5" s="9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>6</v>
@@ -690,8 +684,8 @@
       <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>18</v>
+      <c r="A8" s="11" t="s">
+        <v>16</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -700,7 +694,7 @@
       <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -708,7 +702,7 @@
       <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -716,74 +710,59 @@
       <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>19</v>
+        <v>9</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>20</v>
+        <v>7</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>35</v>
+      <c r="A13" s="12"/>
+      <c r="B13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>28</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>24</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="F13" s="6"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="6"/>
+      <c r="A14" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -794,12 +773,11 @@
     <hyperlink ref="C4" r:id="rId1"/>
     <hyperlink ref="C2" r:id="rId2"/>
     <hyperlink ref="C5" r:id="rId3"/>
-    <hyperlink ref="C14" r:id="rId4"/>
-    <hyperlink ref="C13" r:id="rId5"/>
-    <hyperlink ref="C12" r:id="rId6"/>
-    <hyperlink ref="C11" r:id="rId7"/>
+    <hyperlink ref="C13" r:id="rId4"/>
+    <hyperlink ref="C12" r:id="rId5"/>
+    <hyperlink ref="C11" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>